<commit_message>
fix error in calc 5-year change in ERC
</commit_message>
<xml_diff>
--- a/FullOverride/Report_graphs/RS_tbl.xlsx
+++ b/FullOverride/Report_graphs/RS_tbl.xlsx
@@ -1618,49 +1618,49 @@
         <v>2020.0</v>
       </c>
       <c r="C3" t="n">
-        <v>0.9</v>
+        <v>1.3</v>
       </c>
       <c r="D3" t="n">
         <v>0.0</v>
       </c>
       <c r="E3" t="n">
-        <v>0.9</v>
+        <v>1.3</v>
       </c>
       <c r="F3" t="n">
-        <v>2.6</v>
+        <v>3.15</v>
       </c>
       <c r="G3" t="n">
         <v>0.0</v>
       </c>
       <c r="H3" t="n">
-        <v>2.6</v>
+        <v>3.15</v>
       </c>
       <c r="I3" t="n">
-        <v>3.5</v>
+        <v>4.25</v>
       </c>
       <c r="J3" t="n">
         <v>0.0</v>
       </c>
       <c r="K3" t="n">
-        <v>3.5</v>
+        <v>4.25</v>
       </c>
       <c r="L3" t="n">
-        <v>2.5</v>
+        <v>2.8</v>
       </c>
       <c r="M3" t="n">
         <v>0.0</v>
       </c>
       <c r="N3" t="n">
-        <v>2.5</v>
+        <v>2.8</v>
       </c>
       <c r="O3" t="n">
-        <v>6.9</v>
+        <v>7.35</v>
       </c>
       <c r="P3" t="n">
         <v>0.0</v>
       </c>
       <c r="Q3" t="n">
-        <v>6.9</v>
+        <v>7.35</v>
       </c>
       <c r="R3" t="s">
         <v>26</v>
@@ -1674,49 +1674,49 @@
         <v>2025.0</v>
       </c>
       <c r="C4" t="n">
-        <v>10.3</v>
+        <v>13.4</v>
       </c>
       <c r="D4" t="n">
         <v>0.0</v>
       </c>
       <c r="E4" t="n">
-        <v>9.65</v>
+        <v>13.15</v>
       </c>
       <c r="F4" t="n">
-        <v>14.15</v>
+        <v>19.0</v>
       </c>
       <c r="G4" t="n">
         <v>0.0</v>
       </c>
       <c r="H4" t="n">
-        <v>14.0</v>
+        <v>18.95</v>
       </c>
       <c r="I4" t="n">
-        <v>24.4</v>
+        <v>31.1</v>
       </c>
       <c r="J4" t="n">
         <v>0.0</v>
       </c>
       <c r="K4" t="n">
-        <v>24.1</v>
+        <v>30.95</v>
       </c>
       <c r="L4" t="n">
-        <v>19.3</v>
+        <v>22.95</v>
       </c>
       <c r="M4" t="n">
         <v>0.0</v>
       </c>
       <c r="N4" t="n">
-        <v>18.65</v>
+        <v>22.6</v>
       </c>
       <c r="O4" t="n">
-        <v>27.5</v>
+        <v>29.0</v>
       </c>
       <c r="P4" t="n">
         <v>0.0</v>
       </c>
       <c r="Q4" t="n">
-        <v>26.0</v>
+        <v>27.9</v>
       </c>
       <c r="R4" t="s">
         <v>26</v>
@@ -1730,49 +1730,49 @@
         <v>2030.0</v>
       </c>
       <c r="C5" t="n">
-        <v>18.7</v>
+        <v>23.2</v>
       </c>
       <c r="D5" t="n">
         <v>0.0</v>
       </c>
       <c r="E5" t="n">
-        <v>15.85</v>
+        <v>20.4</v>
       </c>
       <c r="F5" t="n">
-        <v>21.65</v>
+        <v>26.7</v>
       </c>
       <c r="G5" t="n">
         <v>0.0</v>
       </c>
       <c r="H5" t="n">
-        <v>19.6</v>
+        <v>24.9</v>
       </c>
       <c r="I5" t="n">
-        <v>34.05</v>
+        <v>42.7</v>
       </c>
       <c r="J5" t="n">
         <v>0.0</v>
       </c>
       <c r="K5" t="n">
-        <v>32.9</v>
+        <v>41.5</v>
       </c>
       <c r="L5" t="n">
-        <v>32.2</v>
+        <v>37.35</v>
       </c>
       <c r="M5" t="n">
         <v>0.0</v>
       </c>
       <c r="N5" t="n">
-        <v>28.85</v>
+        <v>33.9</v>
       </c>
       <c r="O5" t="n">
-        <v>41.25</v>
+        <v>43.8</v>
       </c>
       <c r="P5" t="n">
         <v>0.0</v>
       </c>
       <c r="Q5" t="n">
-        <v>35.9</v>
+        <v>38.65</v>
       </c>
       <c r="R5" t="s">
         <v>26</v>
@@ -1786,49 +1786,49 @@
         <v>2035.0</v>
       </c>
       <c r="C6" t="n">
-        <v>27.8</v>
+        <v>34.0</v>
       </c>
       <c r="D6" t="n">
         <v>0.0</v>
       </c>
       <c r="E6" t="n">
-        <v>22.6</v>
+        <v>28.5</v>
       </c>
       <c r="F6" t="n">
-        <v>29.75</v>
+        <v>37.35</v>
       </c>
       <c r="G6" t="n">
         <v>0.0</v>
       </c>
       <c r="H6" t="n">
-        <v>26.45</v>
+        <v>33.65</v>
       </c>
       <c r="I6" t="n">
-        <v>40.1</v>
+        <v>50.45</v>
       </c>
       <c r="J6" t="n">
         <v>0.0</v>
       </c>
       <c r="K6" t="n">
-        <v>38.15</v>
+        <v>48.25</v>
       </c>
       <c r="L6" t="n">
-        <v>44.1</v>
+        <v>51.4</v>
       </c>
       <c r="M6" t="n">
         <v>0.0</v>
       </c>
       <c r="N6" t="n">
-        <v>39.35</v>
+        <v>46.1</v>
       </c>
       <c r="O6" t="n">
-        <v>52.55</v>
+        <v>55.75</v>
       </c>
       <c r="P6" t="n">
         <v>0.0</v>
       </c>
       <c r="Q6" t="n">
-        <v>44.9</v>
+        <v>48.4</v>
       </c>
       <c r="R6" t="s">
         <v>26</v>
@@ -1842,49 +1842,49 @@
         <v>2040.0</v>
       </c>
       <c r="C7" t="n">
-        <v>36.15</v>
+        <v>42.6</v>
       </c>
       <c r="D7" t="n">
         <v>0.0</v>
       </c>
       <c r="E7" t="n">
-        <v>28.4</v>
+        <v>34.35</v>
       </c>
       <c r="F7" t="n">
-        <v>36.15</v>
+        <v>44.8</v>
       </c>
       <c r="G7" t="n">
         <v>0.0</v>
       </c>
       <c r="H7" t="n">
-        <v>31.1</v>
+        <v>39.3</v>
       </c>
       <c r="I7" t="n">
-        <v>44.75</v>
+        <v>55.4</v>
       </c>
       <c r="J7" t="n">
         <v>0.0</v>
       </c>
       <c r="K7" t="n">
-        <v>42.0</v>
+        <v>52.3</v>
       </c>
       <c r="L7" t="n">
-        <v>54.6</v>
+        <v>62.0</v>
       </c>
       <c r="M7" t="n">
         <v>0.0</v>
       </c>
       <c r="N7" t="n">
-        <v>47.85</v>
+        <v>54.75</v>
       </c>
       <c r="O7" t="n">
-        <v>60.95</v>
+        <v>63.85</v>
       </c>
       <c r="P7" t="n">
         <v>0.0</v>
       </c>
       <c r="Q7" t="n">
-        <v>51.6</v>
+        <v>54.95</v>
       </c>
       <c r="R7" t="s">
         <v>26</v>
@@ -1898,49 +1898,49 @@
         <v>2044.0</v>
       </c>
       <c r="C8" t="n">
-        <v>40.5</v>
+        <v>47.25</v>
       </c>
       <c r="D8" t="n">
         <v>0.0</v>
       </c>
       <c r="E8" t="n">
-        <v>31.45</v>
+        <v>37.45</v>
       </c>
       <c r="F8" t="n">
-        <v>40.15</v>
+        <v>48.1</v>
       </c>
       <c r="G8" t="n">
         <v>0.0</v>
       </c>
       <c r="H8" t="n">
-        <v>33.45</v>
+        <v>41.45</v>
       </c>
       <c r="I8" t="n">
-        <v>47.35</v>
+        <v>58.0</v>
       </c>
       <c r="J8" t="n">
         <v>0.0</v>
       </c>
       <c r="K8" t="n">
-        <v>43.15</v>
+        <v>53.55</v>
       </c>
       <c r="L8" t="n">
-        <v>59.65</v>
+        <v>66.75</v>
       </c>
       <c r="M8" t="n">
         <v>0.0</v>
       </c>
       <c r="N8" t="n">
-        <v>52.15</v>
+        <v>58.9</v>
       </c>
       <c r="O8" t="n">
-        <v>66.2</v>
+        <v>68.8</v>
       </c>
       <c r="P8" t="n">
         <v>0.0</v>
       </c>
       <c r="Q8" t="n">
-        <v>56.7</v>
+        <v>60.0</v>
       </c>
       <c r="R8" t="s">
         <v>26</v>
@@ -2139,34 +2139,34 @@
         <v>0.0</v>
       </c>
       <c r="H4" t="n">
-        <v>31.45</v>
+        <v>37.45</v>
       </c>
       <c r="I4" t="n">
-        <v>33.45</v>
+        <v>41.45</v>
       </c>
       <c r="J4" t="n">
-        <v>43.15</v>
+        <v>53.55</v>
       </c>
       <c r="K4" t="n">
-        <v>56.7</v>
+        <v>60.0</v>
       </c>
       <c r="L4" t="n">
-        <v>52.15</v>
+        <v>58.9</v>
       </c>
       <c r="M4" t="n">
-        <v>40.5</v>
+        <v>47.25</v>
       </c>
       <c r="N4" t="n">
-        <v>40.15</v>
+        <v>48.1</v>
       </c>
       <c r="O4" t="n">
-        <v>47.35</v>
+        <v>58.0</v>
       </c>
       <c r="P4" t="n">
-        <v>66.2</v>
+        <v>68.8</v>
       </c>
       <c r="Q4" t="n">
-        <v>59.65</v>
+        <v>66.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sd changed to 12%
</commit_message>
<xml_diff>
--- a/FullOverride/Report_graphs/RS_tbl.xlsx
+++ b/FullOverride/Report_graphs/RS_tbl.xlsx
@@ -262,7 +262,7 @@
         <v>0.0</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0</v>
+        <v>0.25</v>
       </c>
       <c r="E3" t="n">
         <v>0.0</v>
@@ -315,7 +315,7 @@
         <v>0.0</v>
       </c>
       <c r="D4" t="n">
-        <v>0.75</v>
+        <v>2.75</v>
       </c>
       <c r="E4" t="n">
         <v>0.0</v>
@@ -368,7 +368,7 @@
         <v>0.0</v>
       </c>
       <c r="D5" t="n">
-        <v>4.0</v>
+        <v>7.9</v>
       </c>
       <c r="E5" t="n">
         <v>0.0</v>
@@ -421,7 +421,7 @@
         <v>0.0</v>
       </c>
       <c r="D6" t="n">
-        <v>8.15</v>
+        <v>14.0</v>
       </c>
       <c r="E6" t="n">
         <v>0.0</v>
@@ -474,7 +474,7 @@
         <v>0.0</v>
       </c>
       <c r="D7" t="n">
-        <v>13.6</v>
+        <v>21.5</v>
       </c>
       <c r="E7" t="n">
         <v>0.0</v>
@@ -527,7 +527,7 @@
         <v>0.05</v>
       </c>
       <c r="D8" t="n">
-        <v>16.75</v>
+        <v>25.45</v>
       </c>
       <c r="E8" t="n">
         <v>0.05</v>
@@ -700,31 +700,31 @@
         <v>2020.0</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0</v>
+        <v>0.1</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0</v>
+        <v>0.3</v>
       </c>
       <c r="E3" t="n">
-        <v>0.0</v>
+        <v>0.1</v>
       </c>
       <c r="F3" t="n">
-        <v>0.05</v>
+        <v>0.25</v>
       </c>
       <c r="G3" t="n">
-        <v>0.2</v>
+        <v>0.65</v>
       </c>
       <c r="H3" t="n">
-        <v>0.05</v>
+        <v>0.25</v>
       </c>
       <c r="I3" t="n">
-        <v>0.05</v>
+        <v>0.4</v>
       </c>
       <c r="J3" t="n">
-        <v>0.25</v>
+        <v>0.85</v>
       </c>
       <c r="K3" t="n">
-        <v>0.05</v>
+        <v>0.4</v>
       </c>
       <c r="L3" t="n">
         <v>0.05</v>
@@ -756,31 +756,31 @@
         <v>2025.0</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0</v>
+        <v>0.55</v>
       </c>
       <c r="D4" t="n">
-        <v>0.85</v>
+        <v>3.1</v>
       </c>
       <c r="E4" t="n">
-        <v>0.0</v>
+        <v>0.55</v>
       </c>
       <c r="F4" t="n">
-        <v>0.25</v>
+        <v>1.2</v>
       </c>
       <c r="G4" t="n">
-        <v>2.35</v>
+        <v>6.9</v>
       </c>
       <c r="H4" t="n">
-        <v>0.25</v>
+        <v>1.15</v>
       </c>
       <c r="I4" t="n">
-        <v>0.8</v>
+        <v>2.8</v>
       </c>
       <c r="J4" t="n">
-        <v>7.7</v>
+        <v>14.45</v>
       </c>
       <c r="K4" t="n">
-        <v>0.75</v>
+        <v>2.8</v>
       </c>
       <c r="L4" t="n">
         <v>0.5</v>
@@ -812,31 +812,31 @@
         <v>2030.0</v>
       </c>
       <c r="C5" t="n">
-        <v>0.05</v>
+        <v>1.2</v>
       </c>
       <c r="D5" t="n">
-        <v>4.55</v>
+        <v>9.15</v>
       </c>
       <c r="E5" t="n">
-        <v>0.05</v>
+        <v>1.15</v>
       </c>
       <c r="F5" t="n">
-        <v>0.3</v>
+        <v>2.2</v>
       </c>
       <c r="G5" t="n">
-        <v>8.35</v>
+        <v>15.2</v>
       </c>
       <c r="H5" t="n">
-        <v>0.3</v>
+        <v>2.15</v>
       </c>
       <c r="I5" t="n">
-        <v>1.6</v>
+        <v>5.2</v>
       </c>
       <c r="J5" t="n">
-        <v>20.05</v>
+        <v>27.5</v>
       </c>
       <c r="K5" t="n">
-        <v>1.55</v>
+        <v>5.15</v>
       </c>
       <c r="L5" t="n">
         <v>1.35</v>
@@ -868,31 +868,31 @@
         <v>2035.0</v>
       </c>
       <c r="C6" t="n">
-        <v>0.1</v>
+        <v>1.85</v>
       </c>
       <c r="D6" t="n">
-        <v>9.45</v>
+        <v>16.05</v>
       </c>
       <c r="E6" t="n">
-        <v>0.1</v>
+        <v>1.8</v>
       </c>
       <c r="F6" t="n">
-        <v>0.35</v>
+        <v>2.8</v>
       </c>
       <c r="G6" t="n">
-        <v>15.25</v>
+        <v>24.2</v>
       </c>
       <c r="H6" t="n">
-        <v>0.35</v>
+        <v>2.7</v>
       </c>
       <c r="I6" t="n">
-        <v>1.95</v>
+        <v>6.35</v>
       </c>
       <c r="J6" t="n">
-        <v>30.6</v>
+        <v>38.65</v>
       </c>
       <c r="K6" t="n">
-        <v>1.9</v>
+        <v>6.25</v>
       </c>
       <c r="L6" t="n">
         <v>2.1</v>
@@ -924,31 +924,31 @@
         <v>2040.0</v>
       </c>
       <c r="C7" t="n">
-        <v>0.2</v>
+        <v>2.55</v>
       </c>
       <c r="D7" t="n">
-        <v>14.7</v>
+        <v>23.85</v>
       </c>
       <c r="E7" t="n">
-        <v>0.2</v>
+        <v>2.5</v>
       </c>
       <c r="F7" t="n">
-        <v>0.45</v>
+        <v>3.45</v>
       </c>
       <c r="G7" t="n">
-        <v>23.15</v>
+        <v>31.05</v>
       </c>
       <c r="H7" t="n">
-        <v>0.45</v>
+        <v>3.35</v>
       </c>
       <c r="I7" t="n">
-        <v>2.1</v>
+        <v>6.95</v>
       </c>
       <c r="J7" t="n">
-        <v>38.2</v>
+        <v>46.6</v>
       </c>
       <c r="K7" t="n">
-        <v>2.05</v>
+        <v>6.85</v>
       </c>
       <c r="L7" t="n">
         <v>2.85</v>
@@ -980,31 +980,31 @@
         <v>2044.0</v>
       </c>
       <c r="C8" t="n">
-        <v>0.25</v>
+        <v>2.8</v>
       </c>
       <c r="D8" t="n">
-        <v>18.1</v>
+        <v>27.95</v>
       </c>
       <c r="E8" t="n">
-        <v>0.25</v>
+        <v>2.65</v>
       </c>
       <c r="F8" t="n">
-        <v>0.5</v>
+        <v>3.75</v>
       </c>
       <c r="G8" t="n">
-        <v>27.25</v>
+        <v>36.3</v>
       </c>
       <c r="H8" t="n">
-        <v>0.5</v>
+        <v>3.6</v>
       </c>
       <c r="I8" t="n">
-        <v>2.15</v>
+        <v>7.05</v>
       </c>
       <c r="J8" t="n">
-        <v>43.9</v>
+        <v>51.1</v>
       </c>
       <c r="K8" t="n">
-        <v>2.1</v>
+        <v>6.95</v>
       </c>
       <c r="L8" t="n">
         <v>3.2</v>
@@ -1159,31 +1159,31 @@
         <v>2020.0</v>
       </c>
       <c r="C3" t="n">
-        <v>1.3</v>
+        <v>2.65</v>
       </c>
       <c r="D3" t="n">
         <v>0.0</v>
       </c>
       <c r="E3" t="n">
-        <v>1.3</v>
+        <v>2.65</v>
       </c>
       <c r="F3" t="n">
-        <v>3.15</v>
+        <v>7.1</v>
       </c>
       <c r="G3" t="n">
         <v>0.0</v>
       </c>
       <c r="H3" t="n">
-        <v>3.15</v>
+        <v>7.1</v>
       </c>
       <c r="I3" t="n">
-        <v>4.25</v>
+        <v>7.95</v>
       </c>
       <c r="J3" t="n">
         <v>0.0</v>
       </c>
       <c r="K3" t="n">
-        <v>4.25</v>
+        <v>7.95</v>
       </c>
       <c r="L3" t="n">
         <v>2.8</v>
@@ -1215,31 +1215,31 @@
         <v>2025.0</v>
       </c>
       <c r="C4" t="n">
-        <v>9.35</v>
+        <v>15.6</v>
       </c>
       <c r="D4" t="n">
         <v>0.0</v>
       </c>
       <c r="E4" t="n">
-        <v>9.3</v>
+        <v>15.6</v>
       </c>
       <c r="F4" t="n">
-        <v>17.9</v>
+        <v>25.15</v>
       </c>
       <c r="G4" t="n">
         <v>0.0</v>
       </c>
       <c r="H4" t="n">
-        <v>17.9</v>
+        <v>25.15</v>
       </c>
       <c r="I4" t="n">
-        <v>29.6</v>
+        <v>35.65</v>
       </c>
       <c r="J4" t="n">
         <v>0.0</v>
       </c>
       <c r="K4" t="n">
-        <v>29.6</v>
+        <v>35.65</v>
       </c>
       <c r="L4" t="n">
         <v>19.3</v>
@@ -1271,31 +1271,31 @@
         <v>2030.0</v>
       </c>
       <c r="C5" t="n">
-        <v>14.3</v>
+        <v>22.7</v>
       </c>
       <c r="D5" t="n">
         <v>0.0</v>
       </c>
       <c r="E5" t="n">
-        <v>14.25</v>
+        <v>22.6</v>
       </c>
       <c r="F5" t="n">
-        <v>23.85</v>
+        <v>32.4</v>
       </c>
       <c r="G5" t="n">
         <v>0.0</v>
       </c>
       <c r="H5" t="n">
-        <v>23.85</v>
+        <v>32.3</v>
       </c>
       <c r="I5" t="n">
-        <v>41.45</v>
+        <v>48.2</v>
       </c>
       <c r="J5" t="n">
         <v>0.0</v>
       </c>
       <c r="K5" t="n">
-        <v>41.4</v>
+        <v>48.15</v>
       </c>
       <c r="L5" t="n">
         <v>29.45</v>
@@ -1327,31 +1327,31 @@
         <v>2035.0</v>
       </c>
       <c r="C6" t="n">
-        <v>18.95</v>
+        <v>29.55</v>
       </c>
       <c r="D6" t="n">
         <v>0.0</v>
       </c>
       <c r="E6" t="n">
-        <v>18.8</v>
+        <v>29.05</v>
       </c>
       <c r="F6" t="n">
-        <v>29.35</v>
+        <v>39.35</v>
       </c>
       <c r="G6" t="n">
         <v>0.0</v>
       </c>
       <c r="H6" t="n">
-        <v>29.25</v>
+        <v>39.2</v>
       </c>
       <c r="I6" t="n">
-        <v>48.45</v>
+        <v>55.45</v>
       </c>
       <c r="J6" t="n">
         <v>0.0</v>
       </c>
       <c r="K6" t="n">
-        <v>48.3</v>
+        <v>55.05</v>
       </c>
       <c r="L6" t="n">
         <v>39.05</v>
@@ -1383,31 +1383,31 @@
         <v>2040.0</v>
       </c>
       <c r="C7" t="n">
-        <v>23.75</v>
+        <v>35.0</v>
       </c>
       <c r="D7" t="n">
         <v>0.0</v>
       </c>
       <c r="E7" t="n">
-        <v>22.85</v>
+        <v>34.05</v>
       </c>
       <c r="F7" t="n">
-        <v>33.35</v>
+        <v>44.15</v>
       </c>
       <c r="G7" t="n">
         <v>0.0</v>
       </c>
       <c r="H7" t="n">
-        <v>33.05</v>
+        <v>43.75</v>
       </c>
       <c r="I7" t="n">
-        <v>52.4</v>
+        <v>59.75</v>
       </c>
       <c r="J7" t="n">
         <v>0.0</v>
       </c>
       <c r="K7" t="n">
-        <v>52.3</v>
+        <v>59.4</v>
       </c>
       <c r="L7" t="n">
         <v>46.5</v>
@@ -1439,31 +1439,31 @@
         <v>2044.0</v>
       </c>
       <c r="C8" t="n">
-        <v>26.35</v>
+        <v>38.35</v>
       </c>
       <c r="D8" t="n">
         <v>0.0</v>
       </c>
       <c r="E8" t="n">
-        <v>25.45</v>
+        <v>36.95</v>
       </c>
       <c r="F8" t="n">
-        <v>35.15</v>
+        <v>46.6</v>
       </c>
       <c r="G8" t="n">
         <v>0.0</v>
       </c>
       <c r="H8" t="n">
-        <v>34.8</v>
+        <v>45.7</v>
       </c>
       <c r="I8" t="n">
-        <v>53.3</v>
+        <v>61.4</v>
       </c>
       <c r="J8" t="n">
         <v>0.0</v>
       </c>
       <c r="K8" t="n">
-        <v>53.2</v>
+        <v>61.0</v>
       </c>
       <c r="L8" t="n">
         <v>50.75</v>
@@ -1618,31 +1618,31 @@
         <v>2020.0</v>
       </c>
       <c r="C3" t="n">
-        <v>1.3</v>
+        <v>2.65</v>
       </c>
       <c r="D3" t="n">
         <v>0.0</v>
       </c>
       <c r="E3" t="n">
-        <v>1.3</v>
+        <v>2.65</v>
       </c>
       <c r="F3" t="n">
-        <v>3.15</v>
+        <v>7.05</v>
       </c>
       <c r="G3" t="n">
         <v>0.0</v>
       </c>
       <c r="H3" t="n">
-        <v>3.15</v>
+        <v>7.05</v>
       </c>
       <c r="I3" t="n">
-        <v>4.25</v>
+        <v>7.95</v>
       </c>
       <c r="J3" t="n">
         <v>0.0</v>
       </c>
       <c r="K3" t="n">
-        <v>4.25</v>
+        <v>7.95</v>
       </c>
       <c r="L3" t="n">
         <v>2.8</v>
@@ -1674,31 +1674,31 @@
         <v>2025.0</v>
       </c>
       <c r="C4" t="n">
-        <v>13.4</v>
+        <v>20.1</v>
       </c>
       <c r="D4" t="n">
         <v>0.0</v>
       </c>
       <c r="E4" t="n">
-        <v>13.15</v>
+        <v>19.25</v>
       </c>
       <c r="F4" t="n">
-        <v>19.0</v>
+        <v>27.25</v>
       </c>
       <c r="G4" t="n">
         <v>0.0</v>
       </c>
       <c r="H4" t="n">
-        <v>18.95</v>
+        <v>27.05</v>
       </c>
       <c r="I4" t="n">
-        <v>31.1</v>
+        <v>38.85</v>
       </c>
       <c r="J4" t="n">
         <v>0.0</v>
       </c>
       <c r="K4" t="n">
-        <v>30.95</v>
+        <v>38.4</v>
       </c>
       <c r="L4" t="n">
         <v>22.95</v>
@@ -1730,31 +1730,31 @@
         <v>2030.0</v>
       </c>
       <c r="C5" t="n">
-        <v>23.2</v>
+        <v>32.7</v>
       </c>
       <c r="D5" t="n">
         <v>0.0</v>
       </c>
       <c r="E5" t="n">
-        <v>20.4</v>
+        <v>28.7</v>
       </c>
       <c r="F5" t="n">
-        <v>26.7</v>
+        <v>38.1</v>
       </c>
       <c r="G5" t="n">
         <v>0.0</v>
       </c>
       <c r="H5" t="n">
-        <v>24.9</v>
+        <v>35.6</v>
       </c>
       <c r="I5" t="n">
-        <v>42.7</v>
+        <v>53.9</v>
       </c>
       <c r="J5" t="n">
         <v>0.0</v>
       </c>
       <c r="K5" t="n">
-        <v>41.5</v>
+        <v>51.7</v>
       </c>
       <c r="L5" t="n">
         <v>37.35</v>
@@ -1786,31 +1786,31 @@
         <v>2035.0</v>
       </c>
       <c r="C6" t="n">
-        <v>34.0</v>
+        <v>45.3</v>
       </c>
       <c r="D6" t="n">
         <v>0.0</v>
       </c>
       <c r="E6" t="n">
-        <v>28.5</v>
+        <v>38.65</v>
       </c>
       <c r="F6" t="n">
-        <v>37.35</v>
+        <v>50.05</v>
       </c>
       <c r="G6" t="n">
         <v>0.0</v>
       </c>
       <c r="H6" t="n">
-        <v>33.65</v>
+        <v>45.35</v>
       </c>
       <c r="I6" t="n">
-        <v>50.45</v>
+        <v>62.7</v>
       </c>
       <c r="J6" t="n">
         <v>0.0</v>
       </c>
       <c r="K6" t="n">
-        <v>48.25</v>
+        <v>59.7</v>
       </c>
       <c r="L6" t="n">
         <v>51.4</v>
@@ -1842,31 +1842,31 @@
         <v>2040.0</v>
       </c>
       <c r="C7" t="n">
-        <v>42.6</v>
+        <v>54.5</v>
       </c>
       <c r="D7" t="n">
         <v>0.0</v>
       </c>
       <c r="E7" t="n">
-        <v>34.35</v>
+        <v>45.45</v>
       </c>
       <c r="F7" t="n">
-        <v>44.8</v>
+        <v>58.2</v>
       </c>
       <c r="G7" t="n">
         <v>0.0</v>
       </c>
       <c r="H7" t="n">
-        <v>39.3</v>
+        <v>51.8</v>
       </c>
       <c r="I7" t="n">
-        <v>55.4</v>
+        <v>67.75</v>
       </c>
       <c r="J7" t="n">
         <v>0.0</v>
       </c>
       <c r="K7" t="n">
-        <v>52.3</v>
+        <v>64.2</v>
       </c>
       <c r="L7" t="n">
         <v>62.0</v>
@@ -1898,31 +1898,31 @@
         <v>2044.0</v>
       </c>
       <c r="C8" t="n">
-        <v>47.25</v>
+        <v>59.55</v>
       </c>
       <c r="D8" t="n">
         <v>0.0</v>
       </c>
       <c r="E8" t="n">
-        <v>37.45</v>
+        <v>49.65</v>
       </c>
       <c r="F8" t="n">
-        <v>48.1</v>
+        <v>62.4</v>
       </c>
       <c r="G8" t="n">
         <v>0.0</v>
       </c>
       <c r="H8" t="n">
-        <v>41.45</v>
+        <v>55.0</v>
       </c>
       <c r="I8" t="n">
-        <v>58.0</v>
+        <v>70.65</v>
       </c>
       <c r="J8" t="n">
         <v>0.0</v>
       </c>
       <c r="K8" t="n">
-        <v>53.55</v>
+        <v>66.3</v>
       </c>
       <c r="L8" t="n">
         <v>66.75</v>
@@ -2018,13 +2018,13 @@
         <v>24</v>
       </c>
       <c r="C2" t="n">
-        <v>18.1</v>
+        <v>27.95</v>
       </c>
       <c r="D2" t="n">
-        <v>27.25</v>
+        <v>36.3</v>
       </c>
       <c r="E2" t="n">
-        <v>43.9</v>
+        <v>51.1</v>
       </c>
       <c r="F2" t="n">
         <v>34.35</v>
@@ -2033,13 +2033,13 @@
         <v>42.8</v>
       </c>
       <c r="H2" t="n">
-        <v>0.25</v>
+        <v>2.65</v>
       </c>
       <c r="I2" t="n">
-        <v>0.5</v>
+        <v>3.6</v>
       </c>
       <c r="J2" t="n">
-        <v>2.1</v>
+        <v>6.95</v>
       </c>
       <c r="K2" t="n">
         <v>11.1</v>
@@ -2048,13 +2048,13 @@
         <v>3.1</v>
       </c>
       <c r="M2" t="n">
-        <v>0.25</v>
+        <v>2.8</v>
       </c>
       <c r="N2" t="n">
-        <v>0.5</v>
+        <v>3.75</v>
       </c>
       <c r="O2" t="n">
-        <v>2.15</v>
+        <v>7.05</v>
       </c>
       <c r="P2" t="n">
         <v>11.6</v>
@@ -2086,13 +2086,13 @@
         <v>0.0</v>
       </c>
       <c r="H3" t="n">
-        <v>25.45</v>
+        <v>36.95</v>
       </c>
       <c r="I3" t="n">
-        <v>34.8</v>
+        <v>45.7</v>
       </c>
       <c r="J3" t="n">
-        <v>53.2</v>
+        <v>61.0</v>
       </c>
       <c r="K3" t="n">
         <v>47.35</v>
@@ -2101,13 +2101,13 @@
         <v>50.05</v>
       </c>
       <c r="M3" t="n">
-        <v>26.35</v>
+        <v>38.35</v>
       </c>
       <c r="N3" t="n">
-        <v>35.15</v>
+        <v>46.6</v>
       </c>
       <c r="O3" t="n">
-        <v>53.3</v>
+        <v>61.4</v>
       </c>
       <c r="P3" t="n">
         <v>49.45</v>
@@ -2139,13 +2139,13 @@
         <v>0.0</v>
       </c>
       <c r="H4" t="n">
-        <v>37.45</v>
+        <v>49.65</v>
       </c>
       <c r="I4" t="n">
-        <v>41.45</v>
+        <v>55.0</v>
       </c>
       <c r="J4" t="n">
-        <v>53.55</v>
+        <v>66.3</v>
       </c>
       <c r="K4" t="n">
         <v>60.0</v>
@@ -2154,13 +2154,13 @@
         <v>58.9</v>
       </c>
       <c r="M4" t="n">
-        <v>47.25</v>
+        <v>59.55</v>
       </c>
       <c r="N4" t="n">
-        <v>48.1</v>
+        <v>62.4</v>
       </c>
       <c r="O4" t="n">
-        <v>58.0</v>
+        <v>70.65</v>
       </c>
       <c r="P4" t="n">
         <v>68.8</v>

</xml_diff>

<commit_message>
update graphs for report
</commit_message>
<xml_diff>
--- a/FullOverride/Report_graphs/RS_tbl.xlsx
+++ b/FullOverride/Report_graphs/RS_tbl.xlsx
@@ -131,10 +131,10 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -143,7 +143,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="true"/>
+    <sheetView tabSelected="true" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>

</xml_diff>